<commit_message>
Added updated triglyceride level analysis
</commit_message>
<xml_diff>
--- a/data/raw/3T3-L1 Cellular Triglyceride Levels.xlsx
+++ b/data/raw/3T3-L1 Cellular Triglyceride Levels.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SPH/Harvey/assays/TG:glycerol assays/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SPH/NS/BridgesLab/Harvey/assays/TG:glycerol assays/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="10820" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Dex following Differentiation</t>
   </si>
@@ -332,11 +332,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-879745936"/>
-        <c:axId val="-879743888"/>
+        <c:axId val="-725522912"/>
+        <c:axId val="-728645008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-879745936"/>
+        <c:axId val="-725522912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -346,7 +346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-879743888"/>
+        <c:crossAx val="-728645008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -354,7 +354,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-879743888"/>
+        <c:axId val="-728645008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -364,7 +364,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-879745936"/>
+        <c:crossAx val="-725522912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -740,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:C10"/>
     </sheetView>
   </sheetViews>
@@ -947,10 +947,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,6 +1032,28 @@
         <v>41851</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1450.3205128205129</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>590.27777777777783</v>
+      </c>
+      <c r="C9" s="1">
+        <v>42972</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>